<commit_message>
test class is added under test folder
</commit_message>
<xml_diff>
--- a/src/main/resources/datafile.xlsx
+++ b/src/main/resources/datafile.xlsx
@@ -62,16 +62,16 @@
     <t>/7</t>
   </si>
   <si>
-    <t>/2</t>
-  </si>
-  <si>
-    <t>{   "firstName": "Arnold",   "lastName": "schengver",   "phoneNumber": "00000099999",   "emailAddress": "jone.mac@thripaty.com" }</t>
-  </si>
-  <si>
-    <t>{   "firstName": "danny",   "lastName": "dannys",   "phoneNumber": "8888899999",   "emailAddress": "jone.mac@thripaty.com" }</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>{   "firstName": "danis",   "lastName": "targerian",   "phoneNumber": "8888899999",   "emailAddress": "jone.mac@thripaty.com" }</t>
+  </si>
+  <si>
+    <t>/3</t>
+  </si>
+  <si>
+    <t>{   "firstName": "stefan",   "lastName": "maclory",   "phoneNumber": "00000099999",   "emailAddress": "jone.mac@marvel.com" }</t>
   </si>
 </sst>
 </file>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -488,19 +488,19 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>